<commit_message>
Research 엑셀의 AnalysisTable 시트 올림
</commit_message>
<xml_diff>
--- a/Excel/Research.xlsx
+++ b/Excel/Research.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65280C61-DDC6-4C44-B8CA-5FFBDBA86AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472AF555-BFF6-4EB2-BA83-FDEF919B91DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A097B07C-A7EB-47A4-9D6C-0246EAD30699}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A097B07C-A7EB-47A4-9D6C-0246EAD30699}"/>
   </bookViews>
   <sheets>
     <sheet name="ResearchTable" sheetId="2" r:id="rId1"/>
+    <sheet name="AnalysisTable" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>level|Int</t>
   </si>
@@ -64,6 +65,42 @@
   </si>
   <si>
     <t>requiredCharacterLevel|Int</t>
+  </si>
+  <si>
+    <t>level|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requiredTime|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requiredAccumulatedTime|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxTime|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>goldBonus|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>originPeriod|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>equipPeriod|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diamondPeriod|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>energyPeriod|Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -429,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F8106D-C533-421C-9D15-EBE282763947}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1565,4 +1602,3416 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219FCC9B-BEF4-452F-99F3-14159C16BC5D}">
+  <dimension ref="A1:I100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <f>3*24*60</f>
+        <v>4320</v>
+      </c>
+      <c r="G2">
+        <f>4*24*60</f>
+        <v>5760</v>
+      </c>
+      <c r="H2">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="I2">
+        <f>2*24*60</f>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f>C2+B3</f>
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">3*24*60</f>
+        <v>4320</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="1">4*24*60</f>
+        <v>5760</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H66" si="2">7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="3">2*24*60</f>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f>C3+B4</f>
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <f>C4+B5</f>
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <f>C5+B6</f>
+        <v>65</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <v>110</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <f>C6+B7</f>
+        <v>105</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>130</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <f>C7+B8</f>
+        <v>155</v>
+      </c>
+      <c r="D8">
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <v>150</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <f>C8+B9</f>
+        <v>215</v>
+      </c>
+      <c r="D9">
+        <v>90</v>
+      </c>
+      <c r="E9">
+        <v>170</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <f>C9+B10</f>
+        <v>285</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
+      </c>
+      <c r="E10">
+        <v>190</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <f>C10+B11</f>
+        <v>365</v>
+      </c>
+      <c r="D11">
+        <f>2*60</f>
+        <v>120</v>
+      </c>
+      <c r="E11">
+        <v>210</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>90</v>
+      </c>
+      <c r="C12">
+        <f>C11+B12</f>
+        <v>455</v>
+      </c>
+      <c r="D12">
+        <v>120</v>
+      </c>
+      <c r="E12">
+        <v>230</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <f>C12+B13</f>
+        <v>555</v>
+      </c>
+      <c r="D13">
+        <v>120</v>
+      </c>
+      <c r="E13">
+        <v>250</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>110</v>
+      </c>
+      <c r="C14">
+        <f>C13+B14</f>
+        <v>665</v>
+      </c>
+      <c r="D14">
+        <v>120</v>
+      </c>
+      <c r="E14">
+        <v>270</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>120</v>
+      </c>
+      <c r="C15">
+        <f>C14+B15</f>
+        <v>785</v>
+      </c>
+      <c r="D15">
+        <v>120</v>
+      </c>
+      <c r="E15">
+        <v>290</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>130</v>
+      </c>
+      <c r="C16">
+        <f>C15+B16</f>
+        <v>915</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <v>310</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>140</v>
+      </c>
+      <c r="C17">
+        <f>C16+B17</f>
+        <v>1055</v>
+      </c>
+      <c r="D17">
+        <v>120</v>
+      </c>
+      <c r="E17">
+        <v>330</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <f>C17+B18</f>
+        <v>1205</v>
+      </c>
+      <c r="D18">
+        <v>120</v>
+      </c>
+      <c r="E18">
+        <v>350</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>160</v>
+      </c>
+      <c r="C19">
+        <f>C18+B19</f>
+        <v>1365</v>
+      </c>
+      <c r="D19">
+        <v>120</v>
+      </c>
+      <c r="E19">
+        <v>370</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>170</v>
+      </c>
+      <c r="C20">
+        <f>C19+B20</f>
+        <v>1535</v>
+      </c>
+      <c r="D20">
+        <v>120</v>
+      </c>
+      <c r="E20">
+        <v>390</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>180</v>
+      </c>
+      <c r="C21">
+        <f>C20+B21</f>
+        <v>1715</v>
+      </c>
+      <c r="D21">
+        <f>3*60</f>
+        <v>180</v>
+      </c>
+      <c r="E21">
+        <v>410</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>190</v>
+      </c>
+      <c r="C22">
+        <f>C21+B22</f>
+        <v>1905</v>
+      </c>
+      <c r="D22">
+        <v>180</v>
+      </c>
+      <c r="E22">
+        <v>430</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>200</v>
+      </c>
+      <c r="C23">
+        <f>C22+B23</f>
+        <v>2105</v>
+      </c>
+      <c r="D23">
+        <v>180</v>
+      </c>
+      <c r="E23">
+        <v>450</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>210</v>
+      </c>
+      <c r="C24">
+        <f>C23+B24</f>
+        <v>2315</v>
+      </c>
+      <c r="D24">
+        <v>180</v>
+      </c>
+      <c r="E24">
+        <v>470</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>220</v>
+      </c>
+      <c r="C25">
+        <f>C24+B25</f>
+        <v>2535</v>
+      </c>
+      <c r="D25">
+        <v>180</v>
+      </c>
+      <c r="E25">
+        <v>490</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>230</v>
+      </c>
+      <c r="C26">
+        <f>C25+B26</f>
+        <v>2765</v>
+      </c>
+      <c r="D26">
+        <v>180</v>
+      </c>
+      <c r="E26">
+        <v>510</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>240</v>
+      </c>
+      <c r="C27">
+        <f>C26+B27</f>
+        <v>3005</v>
+      </c>
+      <c r="D27">
+        <v>180</v>
+      </c>
+      <c r="E27">
+        <v>530</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>250</v>
+      </c>
+      <c r="C28">
+        <f>C27+B28</f>
+        <v>3255</v>
+      </c>
+      <c r="D28">
+        <v>180</v>
+      </c>
+      <c r="E28">
+        <v>550</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>260</v>
+      </c>
+      <c r="C29">
+        <f>C28+B29</f>
+        <v>3515</v>
+      </c>
+      <c r="D29">
+        <v>180</v>
+      </c>
+      <c r="E29">
+        <v>570</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>270</v>
+      </c>
+      <c r="C30">
+        <f>C29+B30</f>
+        <v>3785</v>
+      </c>
+      <c r="D30">
+        <v>180</v>
+      </c>
+      <c r="E30">
+        <v>590</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>280</v>
+      </c>
+      <c r="C31">
+        <f>C30+B31</f>
+        <v>4065</v>
+      </c>
+      <c r="D31">
+        <f>4*60</f>
+        <v>240</v>
+      </c>
+      <c r="E31">
+        <v>610</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>290</v>
+      </c>
+      <c r="C32">
+        <f>C31+B32</f>
+        <v>4355</v>
+      </c>
+      <c r="D32">
+        <v>240</v>
+      </c>
+      <c r="E32">
+        <v>630</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>300</v>
+      </c>
+      <c r="C33">
+        <f>C32+B33</f>
+        <v>4655</v>
+      </c>
+      <c r="D33">
+        <v>240</v>
+      </c>
+      <c r="E33">
+        <v>650</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>310</v>
+      </c>
+      <c r="C34">
+        <f>C33+B34</f>
+        <v>4965</v>
+      </c>
+      <c r="D34">
+        <v>240</v>
+      </c>
+      <c r="E34">
+        <v>670</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>320</v>
+      </c>
+      <c r="C35">
+        <f>C34+B35</f>
+        <v>5285</v>
+      </c>
+      <c r="D35">
+        <v>240</v>
+      </c>
+      <c r="E35">
+        <v>690</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>330</v>
+      </c>
+      <c r="C36">
+        <f>C35+B36</f>
+        <v>5615</v>
+      </c>
+      <c r="D36">
+        <v>240</v>
+      </c>
+      <c r="E36">
+        <v>710</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>340</v>
+      </c>
+      <c r="C37">
+        <f>C36+B37</f>
+        <v>5955</v>
+      </c>
+      <c r="D37">
+        <v>240</v>
+      </c>
+      <c r="E37">
+        <v>730</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>350</v>
+      </c>
+      <c r="C38">
+        <f>C37+B38</f>
+        <v>6305</v>
+      </c>
+      <c r="D38">
+        <v>240</v>
+      </c>
+      <c r="E38">
+        <v>750</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>360</v>
+      </c>
+      <c r="C39">
+        <f>C38+B39</f>
+        <v>6665</v>
+      </c>
+      <c r="D39">
+        <v>240</v>
+      </c>
+      <c r="E39">
+        <v>770</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>370</v>
+      </c>
+      <c r="C40">
+        <f>C39+B40</f>
+        <v>7035</v>
+      </c>
+      <c r="D40">
+        <v>240</v>
+      </c>
+      <c r="E40">
+        <v>790</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>380</v>
+      </c>
+      <c r="C41">
+        <f>C40+B41</f>
+        <v>7415</v>
+      </c>
+      <c r="D41">
+        <v>360</v>
+      </c>
+      <c r="E41">
+        <v>810</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>390</v>
+      </c>
+      <c r="C42">
+        <f>C41+B42</f>
+        <v>7805</v>
+      </c>
+      <c r="D42">
+        <v>360</v>
+      </c>
+      <c r="E42">
+        <v>830</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>400</v>
+      </c>
+      <c r="C43">
+        <f>C42+B43</f>
+        <v>8205</v>
+      </c>
+      <c r="D43">
+        <v>360</v>
+      </c>
+      <c r="E43">
+        <v>850</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>410</v>
+      </c>
+      <c r="C44">
+        <f>C43+B44</f>
+        <v>8615</v>
+      </c>
+      <c r="D44">
+        <v>360</v>
+      </c>
+      <c r="E44">
+        <v>870</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>420</v>
+      </c>
+      <c r="C45">
+        <f>C44+B45</f>
+        <v>9035</v>
+      </c>
+      <c r="D45">
+        <v>360</v>
+      </c>
+      <c r="E45">
+        <v>890</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>430</v>
+      </c>
+      <c r="C46">
+        <f>C45+B46</f>
+        <v>9465</v>
+      </c>
+      <c r="D46">
+        <v>360</v>
+      </c>
+      <c r="E46">
+        <v>910</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>440</v>
+      </c>
+      <c r="C47">
+        <f>C46+B47</f>
+        <v>9905</v>
+      </c>
+      <c r="D47">
+        <v>360</v>
+      </c>
+      <c r="E47">
+        <v>930</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>450</v>
+      </c>
+      <c r="C48">
+        <f>C47+B48</f>
+        <v>10355</v>
+      </c>
+      <c r="D48">
+        <v>360</v>
+      </c>
+      <c r="E48">
+        <v>950</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>460</v>
+      </c>
+      <c r="C49">
+        <f>C48+B49</f>
+        <v>10815</v>
+      </c>
+      <c r="D49">
+        <v>360</v>
+      </c>
+      <c r="E49">
+        <v>970</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>470</v>
+      </c>
+      <c r="C50">
+        <f>C49+B50</f>
+        <v>11285</v>
+      </c>
+      <c r="D50">
+        <v>360</v>
+      </c>
+      <c r="E50">
+        <v>990</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>480</v>
+      </c>
+      <c r="C51">
+        <f>C50+B51</f>
+        <v>11765</v>
+      </c>
+      <c r="D51">
+        <v>480</v>
+      </c>
+      <c r="E51">
+        <v>1010</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>490</v>
+      </c>
+      <c r="C52">
+        <f>C51+B52</f>
+        <v>12255</v>
+      </c>
+      <c r="D52">
+        <v>480</v>
+      </c>
+      <c r="E52">
+        <v>1030</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>500</v>
+      </c>
+      <c r="C53">
+        <f>C52+B53</f>
+        <v>12755</v>
+      </c>
+      <c r="D53">
+        <v>480</v>
+      </c>
+      <c r="E53">
+        <v>1050</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>510</v>
+      </c>
+      <c r="C54">
+        <f>C53+B54</f>
+        <v>13265</v>
+      </c>
+      <c r="D54">
+        <v>480</v>
+      </c>
+      <c r="E54">
+        <v>1070</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>520</v>
+      </c>
+      <c r="C55">
+        <f>C54+B55</f>
+        <v>13785</v>
+      </c>
+      <c r="D55">
+        <v>480</v>
+      </c>
+      <c r="E55">
+        <v>1090</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>530</v>
+      </c>
+      <c r="C56">
+        <f>C55+B56</f>
+        <v>14315</v>
+      </c>
+      <c r="D56">
+        <v>480</v>
+      </c>
+      <c r="E56">
+        <v>1110</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>540</v>
+      </c>
+      <c r="C57">
+        <f>C56+B57</f>
+        <v>14855</v>
+      </c>
+      <c r="D57">
+        <v>480</v>
+      </c>
+      <c r="E57">
+        <v>1130</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>550</v>
+      </c>
+      <c r="C58">
+        <f>C57+B58</f>
+        <v>15405</v>
+      </c>
+      <c r="D58">
+        <v>480</v>
+      </c>
+      <c r="E58">
+        <v>1150</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>560</v>
+      </c>
+      <c r="C59">
+        <f>C58+B59</f>
+        <v>15965</v>
+      </c>
+      <c r="D59">
+        <v>480</v>
+      </c>
+      <c r="E59">
+        <v>1170</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>570</v>
+      </c>
+      <c r="C60">
+        <f>C59+B60</f>
+        <v>16535</v>
+      </c>
+      <c r="D60">
+        <v>480</v>
+      </c>
+      <c r="E60">
+        <v>1190</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>580</v>
+      </c>
+      <c r="C61">
+        <f>C60+B61</f>
+        <v>17115</v>
+      </c>
+      <c r="D61">
+        <v>600</v>
+      </c>
+      <c r="E61">
+        <v>1210</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>590</v>
+      </c>
+      <c r="C62">
+        <f>C61+B62</f>
+        <v>17705</v>
+      </c>
+      <c r="D62">
+        <v>600</v>
+      </c>
+      <c r="E62">
+        <v>1230</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>600</v>
+      </c>
+      <c r="C63">
+        <f>C62+B63</f>
+        <v>18305</v>
+      </c>
+      <c r="D63">
+        <v>600</v>
+      </c>
+      <c r="E63">
+        <v>1250</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>610</v>
+      </c>
+      <c r="C64">
+        <f>C63+B64</f>
+        <v>18915</v>
+      </c>
+      <c r="D64">
+        <v>600</v>
+      </c>
+      <c r="E64">
+        <v>1270</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>620</v>
+      </c>
+      <c r="C65">
+        <f>C64+B65</f>
+        <v>19535</v>
+      </c>
+      <c r="D65">
+        <v>600</v>
+      </c>
+      <c r="E65">
+        <v>1290</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>630</v>
+      </c>
+      <c r="C66">
+        <f>C65+B66</f>
+        <v>20165</v>
+      </c>
+      <c r="D66">
+        <v>600</v>
+      </c>
+      <c r="E66">
+        <v>1310</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>5760</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="2"/>
+        <v>10080</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="3"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>640</v>
+      </c>
+      <c r="C67">
+        <f>C66+B67</f>
+        <v>20805</v>
+      </c>
+      <c r="D67">
+        <v>600</v>
+      </c>
+      <c r="E67">
+        <v>1330</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F100" si="4">3*24*60</f>
+        <v>4320</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G100" si="5">4*24*60</f>
+        <v>5760</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H100" si="6">7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I100" si="7">2*24*60</f>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>650</v>
+      </c>
+      <c r="C68">
+        <f>C67+B68</f>
+        <v>21455</v>
+      </c>
+      <c r="D68">
+        <v>600</v>
+      </c>
+      <c r="E68">
+        <v>1350</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>660</v>
+      </c>
+      <c r="C69">
+        <f>C68+B69</f>
+        <v>22115</v>
+      </c>
+      <c r="D69">
+        <v>600</v>
+      </c>
+      <c r="E69">
+        <v>1370</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>670</v>
+      </c>
+      <c r="C70">
+        <f>C69+B70</f>
+        <v>22785</v>
+      </c>
+      <c r="D70">
+        <v>600</v>
+      </c>
+      <c r="E70">
+        <v>1390</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>680</v>
+      </c>
+      <c r="C71">
+        <f>C70+B71</f>
+        <v>23465</v>
+      </c>
+      <c r="D71">
+        <v>720</v>
+      </c>
+      <c r="E71">
+        <v>1410</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>690</v>
+      </c>
+      <c r="C72">
+        <f>C71+B72</f>
+        <v>24155</v>
+      </c>
+      <c r="D72">
+        <v>720</v>
+      </c>
+      <c r="E72">
+        <v>1430</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>700</v>
+      </c>
+      <c r="C73">
+        <f>C72+B73</f>
+        <v>24855</v>
+      </c>
+      <c r="D73">
+        <v>720</v>
+      </c>
+      <c r="E73">
+        <v>1450</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>710</v>
+      </c>
+      <c r="C74">
+        <f>C73+B74</f>
+        <v>25565</v>
+      </c>
+      <c r="D74">
+        <v>720</v>
+      </c>
+      <c r="E74">
+        <v>1470</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>720</v>
+      </c>
+      <c r="C75">
+        <f>C74+B75</f>
+        <v>26285</v>
+      </c>
+      <c r="D75">
+        <v>720</v>
+      </c>
+      <c r="E75">
+        <v>1490</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>730</v>
+      </c>
+      <c r="C76">
+        <f>C75+B76</f>
+        <v>27015</v>
+      </c>
+      <c r="D76">
+        <v>720</v>
+      </c>
+      <c r="E76">
+        <v>1510</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>740</v>
+      </c>
+      <c r="C77">
+        <f>C76+B77</f>
+        <v>27755</v>
+      </c>
+      <c r="D77">
+        <v>720</v>
+      </c>
+      <c r="E77">
+        <v>1530</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>750</v>
+      </c>
+      <c r="C78">
+        <f>C77+B78</f>
+        <v>28505</v>
+      </c>
+      <c r="D78">
+        <v>720</v>
+      </c>
+      <c r="E78">
+        <v>1550</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>760</v>
+      </c>
+      <c r="C79">
+        <f>C78+B79</f>
+        <v>29265</v>
+      </c>
+      <c r="D79">
+        <v>720</v>
+      </c>
+      <c r="E79">
+        <v>1570</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>770</v>
+      </c>
+      <c r="C80">
+        <f>C79+B80</f>
+        <v>30035</v>
+      </c>
+      <c r="D80">
+        <v>720</v>
+      </c>
+      <c r="E80">
+        <v>1590</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>780</v>
+      </c>
+      <c r="C81">
+        <f>C80+B81</f>
+        <v>30815</v>
+      </c>
+      <c r="D81">
+        <v>840</v>
+      </c>
+      <c r="E81">
+        <v>1610</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>790</v>
+      </c>
+      <c r="C82">
+        <f>C81+B82</f>
+        <v>31605</v>
+      </c>
+      <c r="D82">
+        <v>840</v>
+      </c>
+      <c r="E82">
+        <v>1630</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>800</v>
+      </c>
+      <c r="C83">
+        <f>C82+B83</f>
+        <v>32405</v>
+      </c>
+      <c r="D83">
+        <v>840</v>
+      </c>
+      <c r="E83">
+        <v>1650</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>810</v>
+      </c>
+      <c r="C84">
+        <f>C83+B84</f>
+        <v>33215</v>
+      </c>
+      <c r="D84">
+        <v>840</v>
+      </c>
+      <c r="E84">
+        <v>1670</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>820</v>
+      </c>
+      <c r="C85">
+        <f>C84+B85</f>
+        <v>34035</v>
+      </c>
+      <c r="D85">
+        <v>840</v>
+      </c>
+      <c r="E85">
+        <v>1690</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>830</v>
+      </c>
+      <c r="C86">
+        <f>C85+B86</f>
+        <v>34865</v>
+      </c>
+      <c r="D86">
+        <v>840</v>
+      </c>
+      <c r="E86">
+        <v>1710</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>840</v>
+      </c>
+      <c r="C87">
+        <f>C86+B87</f>
+        <v>35705</v>
+      </c>
+      <c r="D87">
+        <v>840</v>
+      </c>
+      <c r="E87">
+        <v>1730</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>850</v>
+      </c>
+      <c r="C88">
+        <f>C87+B88</f>
+        <v>36555</v>
+      </c>
+      <c r="D88">
+        <v>840</v>
+      </c>
+      <c r="E88">
+        <v>1750</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>860</v>
+      </c>
+      <c r="C89">
+        <f>C88+B89</f>
+        <v>37415</v>
+      </c>
+      <c r="D89">
+        <v>840</v>
+      </c>
+      <c r="E89">
+        <v>1770</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>870</v>
+      </c>
+      <c r="C90">
+        <f>C89+B90</f>
+        <v>38285</v>
+      </c>
+      <c r="D90">
+        <v>840</v>
+      </c>
+      <c r="E90">
+        <v>1790</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>880</v>
+      </c>
+      <c r="C91">
+        <f>C90+B91</f>
+        <v>39165</v>
+      </c>
+      <c r="D91">
+        <v>960</v>
+      </c>
+      <c r="E91">
+        <v>1810</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>890</v>
+      </c>
+      <c r="C92">
+        <f>C91+B92</f>
+        <v>40055</v>
+      </c>
+      <c r="D92">
+        <v>960</v>
+      </c>
+      <c r="E92">
+        <v>1830</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>900</v>
+      </c>
+      <c r="C93">
+        <f>C92+B93</f>
+        <v>40955</v>
+      </c>
+      <c r="D93">
+        <v>960</v>
+      </c>
+      <c r="E93">
+        <v>1850</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>910</v>
+      </c>
+      <c r="C94">
+        <f>C93+B94</f>
+        <v>41865</v>
+      </c>
+      <c r="D94">
+        <v>960</v>
+      </c>
+      <c r="E94">
+        <v>1870</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>920</v>
+      </c>
+      <c r="C95">
+        <f>C94+B95</f>
+        <v>42785</v>
+      </c>
+      <c r="D95">
+        <v>960</v>
+      </c>
+      <c r="E95">
+        <v>1890</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>930</v>
+      </c>
+      <c r="C96">
+        <f>C95+B96</f>
+        <v>43715</v>
+      </c>
+      <c r="D96">
+        <v>960</v>
+      </c>
+      <c r="E96">
+        <v>1910</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>940</v>
+      </c>
+      <c r="C97">
+        <f>C96+B97</f>
+        <v>44655</v>
+      </c>
+      <c r="D97">
+        <v>960</v>
+      </c>
+      <c r="E97">
+        <v>1930</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>950</v>
+      </c>
+      <c r="C98">
+        <f>C97+B98</f>
+        <v>45605</v>
+      </c>
+      <c r="D98">
+        <v>960</v>
+      </c>
+      <c r="E98">
+        <v>1950</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>960</v>
+      </c>
+      <c r="C99">
+        <f>C98+B99</f>
+        <v>46565</v>
+      </c>
+      <c r="D99">
+        <v>960</v>
+      </c>
+      <c r="E99">
+        <v>1970</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>970</v>
+      </c>
+      <c r="C100">
+        <f>C99+B100</f>
+        <v>47535</v>
+      </c>
+      <c r="D100">
+        <v>960</v>
+      </c>
+      <c r="E100">
+        <v>1990</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="4"/>
+        <v>4320</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="5"/>
+        <v>5760</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="6"/>
+        <v>10080</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="7"/>
+        <v>2880</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
45 => 59 로 확장
</commit_message>
<xml_diff>
--- a/Excel/Research.xlsx
+++ b/Excel/Research.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C77705-2CDE-405B-BEF8-C5EB6510D962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4C525C-216A-4EA7-AB54-BD68C43271A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A097B07C-A7EB-47A4-9D6C-0246EAD30699}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A097B07C-A7EB-47A4-9D6C-0246EAD30699}"/>
   </bookViews>
   <sheets>
     <sheet name="ResearchTable" sheetId="2" r:id="rId1"/>
     <sheet name="AnalysisTable" sheetId="3" r:id="rId2"/>
     <sheet name="AnalysisKeyTable" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -465,9 +468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F8106D-C533-421C-9D15-EBE282763947}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1597,6 +1602,337 @@
       </c>
       <c r="K46">
         <v>1275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>272</v>
+      </c>
+      <c r="F47">
+        <v>17500</v>
+      </c>
+      <c r="I47">
+        <v>25</v>
+      </c>
+      <c r="J47">
+        <v>12150</v>
+      </c>
+      <c r="K47">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>283</v>
+      </c>
+      <c r="F48">
+        <v>17900</v>
+      </c>
+      <c r="H48">
+        <v>25</v>
+      </c>
+      <c r="I48">
+        <v>15</v>
+      </c>
+      <c r="J48">
+        <v>13450</v>
+      </c>
+      <c r="K48">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>295</v>
+      </c>
+      <c r="F49">
+        <v>17300</v>
+      </c>
+      <c r="H49">
+        <v>30</v>
+      </c>
+      <c r="J49">
+        <v>15250</v>
+      </c>
+      <c r="K49">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>302</v>
+      </c>
+      <c r="F50">
+        <v>18200</v>
+      </c>
+      <c r="I50">
+        <v>20</v>
+      </c>
+      <c r="J50">
+        <v>15250</v>
+      </c>
+      <c r="K50">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>310</v>
+      </c>
+      <c r="F51">
+        <v>18500</v>
+      </c>
+      <c r="H51">
+        <v>35</v>
+      </c>
+      <c r="J51">
+        <v>17150</v>
+      </c>
+      <c r="K51">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>319</v>
+      </c>
+      <c r="F52">
+        <v>41000</v>
+      </c>
+      <c r="G52">
+        <v>55</v>
+      </c>
+      <c r="J52">
+        <v>17150</v>
+      </c>
+      <c r="K52">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>329</v>
+      </c>
+      <c r="F53">
+        <v>23200</v>
+      </c>
+      <c r="H53">
+        <v>25</v>
+      </c>
+      <c r="I53">
+        <v>20</v>
+      </c>
+      <c r="J53">
+        <v>18750</v>
+      </c>
+      <c r="K53">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>338</v>
+      </c>
+      <c r="F54">
+        <v>23000</v>
+      </c>
+      <c r="H54">
+        <v>30</v>
+      </c>
+      <c r="J54">
+        <v>20550</v>
+      </c>
+      <c r="K54">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>348</v>
+      </c>
+      <c r="F55">
+        <v>22700</v>
+      </c>
+      <c r="I55">
+        <v>25</v>
+      </c>
+      <c r="J55">
+        <v>20550</v>
+      </c>
+      <c r="K55">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>357</v>
+      </c>
+      <c r="F56">
+        <v>23200</v>
+      </c>
+      <c r="H56">
+        <v>30</v>
+      </c>
+      <c r="J56">
+        <v>22550</v>
+      </c>
+      <c r="K56">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>368</v>
+      </c>
+      <c r="F57">
+        <v>24000</v>
+      </c>
+      <c r="H57">
+        <v>25</v>
+      </c>
+      <c r="I57">
+        <v>15</v>
+      </c>
+      <c r="J57">
+        <v>24350</v>
+      </c>
+      <c r="K57">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>378</v>
+      </c>
+      <c r="F58">
+        <v>23500</v>
+      </c>
+      <c r="H58">
+        <v>30</v>
+      </c>
+      <c r="J58">
+        <v>26550</v>
+      </c>
+      <c r="K58">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>389</v>
+      </c>
+      <c r="F59">
+        <v>23800</v>
+      </c>
+      <c r="I59">
+        <v>20</v>
+      </c>
+      <c r="J59">
+        <v>26550</v>
+      </c>
+      <c r="K59">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>399</v>
+      </c>
+      <c r="F60">
+        <v>52000</v>
+      </c>
+      <c r="G60">
+        <v>50</v>
+      </c>
+      <c r="J60">
+        <v>26550</v>
+      </c>
+      <c r="K60">
+        <v>3015</v>
       </c>
     </row>
   </sheetData>
@@ -1609,7 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219FCC9B-BEF4-452F-99F3-14159C16BC5D}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>